<commit_message>
[Add] : FrontEnd Prototype
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Báo Cáo Team/General/meeting_grant.xlsx
+++ b/ToDoApp-Doc/Báo Cáo Team/General/meeting_grant.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ToDoApp\Báo Cáo Team\General\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\To-Do-App\ToDoApp-Doc\Báo Cáo Team\General\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Offline 1</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>15/10/2020</t>
+  </si>
+  <si>
+    <t>Offline 7</t>
+  </si>
+  <si>
+    <t>17/10/2020</t>
   </si>
 </sst>
 </file>
@@ -228,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -271,10 +277,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -560,7 +575,7 @@
   <dimension ref="A2:N12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,30 +740,53 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="3">
         <v>2</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="21"/>
       <c r="N8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="10">
+        <v>6</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="1">
+        <v>5</v>
+      </c>
+    </row>
     <row r="10" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[Add]: New Activity Bar Chart
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Báo Cáo Team/General/meeting_grant.xlsx
+++ b/ToDoApp-Doc/Báo Cáo Team/General/meeting_grant.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Offline 1</t>
   </si>
@@ -84,13 +84,70 @@
   </si>
   <si>
     <t>17/10/2020</t>
+  </si>
+  <si>
+    <t>Offline 8</t>
+  </si>
+  <si>
+    <t>Offline 9</t>
+  </si>
+  <si>
+    <t>22/10/2020</t>
+  </si>
+  <si>
+    <t>MEETING STATISTICS</t>
+  </si>
+  <si>
+    <t>Online 1</t>
+  </si>
+  <si>
+    <t>21/10/2020</t>
+  </si>
+  <si>
+    <t>Tên Buổi Họp</t>
+  </si>
+  <si>
+    <t>Thời Lượng</t>
+  </si>
+  <si>
+    <t>Ngày Họp</t>
+  </si>
+  <si>
+    <t>Đánh Giá Chất Lượng</t>
+  </si>
+  <si>
+    <t>23/10/2020</t>
+  </si>
+  <si>
+    <t>Offline 10</t>
+  </si>
+  <si>
+    <t>24/10/2020</t>
+  </si>
+  <si>
+    <t>Online 2</t>
+  </si>
+  <si>
+    <t>Offline 11</t>
+  </si>
+  <si>
+    <t>27/10/2020</t>
+  </si>
+  <si>
+    <t>28/10/2020</t>
+  </si>
+  <si>
+    <t>Offline 12</t>
+  </si>
+  <si>
+    <t>29/10/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +166,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="32"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Roboto Mono"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -176,30 +247,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -234,50 +283,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -289,8 +318,53 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,225 +646,424 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N12"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="14" width="12.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="15" width="12.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14" t="s">
+    <row r="1" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N3" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B4" s="18">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="1">
+      <c r="D4" s="16">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="18">
         <v>6</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C5" s="19">
         <v>43900</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="1">
+      <c r="D5" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="18">
         <v>2</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C6" s="19">
         <v>44053</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="1">
+      <c r="D6" s="16">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B7" s="18">
         <v>2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C7" s="19">
         <v>44094</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="1">
+      <c r="D7" s="16">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B8" s="18">
         <v>6</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C8" s="19">
         <v>44114</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="1">
+      <c r="D8" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="18">
         <v>2</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="1">
+      <c r="D9" s="16">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B10" s="18">
         <v>6</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="1">
+      <c r="D10" s="16">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="12"/>
+    </row>
+    <row r="11" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="16">
+        <v>6.5</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="16">
+        <v>4.5</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="11"/>
+    </row>
+    <row r="13" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="18">
+        <v>2</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="27">
+        <v>4</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="12"/>
+    </row>
+    <row r="14" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="18">
+        <v>6</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="27">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="12"/>
+    </row>
+    <row r="15" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="18">
+        <v>5</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="27">
+        <v>7</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="12"/>
+    </row>
+    <row r="16" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="18">
+        <v>2</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="27">
+        <v>6</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="22">
+        <v>2</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="24">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>SUM(B4:B17)</f>
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[Document, Modified] : TaskList(1) & MyMusic UseCase Specification
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Báo Cáo Team/General/meeting_grant.xlsx
+++ b/ToDoApp-Doc/Báo Cáo Team/General/meeting_grant.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Offline 1</t>
   </si>
@@ -84,13 +84,70 @@
   </si>
   <si>
     <t>17/10/2020</t>
+  </si>
+  <si>
+    <t>Offline 8</t>
+  </si>
+  <si>
+    <t>Offline 9</t>
+  </si>
+  <si>
+    <t>22/10/2020</t>
+  </si>
+  <si>
+    <t>MEETING STATISTICS</t>
+  </si>
+  <si>
+    <t>Online 1</t>
+  </si>
+  <si>
+    <t>21/10/2020</t>
+  </si>
+  <si>
+    <t>Tên Buổi Họp</t>
+  </si>
+  <si>
+    <t>Thời Lượng</t>
+  </si>
+  <si>
+    <t>Ngày Họp</t>
+  </si>
+  <si>
+    <t>Đánh Giá Chất Lượng</t>
+  </si>
+  <si>
+    <t>23/10/2020</t>
+  </si>
+  <si>
+    <t>Offline 10</t>
+  </si>
+  <si>
+    <t>24/10/2020</t>
+  </si>
+  <si>
+    <t>Online 2</t>
+  </si>
+  <si>
+    <t>Offline 11</t>
+  </si>
+  <si>
+    <t>27/10/2020</t>
+  </si>
+  <si>
+    <t>28/10/2020</t>
+  </si>
+  <si>
+    <t>Offline 12</t>
+  </si>
+  <si>
+    <t>29/10/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +166,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="32"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Roboto Mono"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -176,30 +247,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -234,50 +283,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -289,8 +318,53 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,225 +646,424 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N12"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="14" width="12.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="15" width="12.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14" t="s">
+    <row r="1" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N3" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B4" s="18">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="1">
+      <c r="D4" s="16">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="18">
         <v>6</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C5" s="19">
         <v>43900</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="1">
+      <c r="D5" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="18">
         <v>2</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C6" s="19">
         <v>44053</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="1">
+      <c r="D6" s="16">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B7" s="18">
         <v>2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C7" s="19">
         <v>44094</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="1">
+      <c r="D7" s="16">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B8" s="18">
         <v>6</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C8" s="19">
         <v>44114</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="1">
+      <c r="D8" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="18">
         <v>2</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="1">
+      <c r="D9" s="16">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B10" s="18">
         <v>6</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="1">
+      <c r="D10" s="16">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="12"/>
+    </row>
+    <row r="11" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="16">
+        <v>6.5</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="16">
+        <v>4.5</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="11"/>
+    </row>
+    <row r="13" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="18">
+        <v>2</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="27">
+        <v>4</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="12"/>
+    </row>
+    <row r="14" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="18">
+        <v>6</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="27">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="12"/>
+    </row>
+    <row r="15" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="18">
+        <v>5</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="27">
+        <v>7</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="12"/>
+    </row>
+    <row r="16" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="18">
+        <v>2</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="27">
+        <v>6</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="22">
+        <v>2</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="24">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>SUM(B4:B17)</f>
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[Modified] Meeting Bar Chart
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Báo Cáo Team/General/meeting_grant.xlsx
+++ b/ToDoApp-Doc/Báo Cáo Team/General/meeting_grant.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Offline 1</t>
   </si>
@@ -147,6 +147,21 @@
   </si>
   <si>
     <t>31/10/2020</t>
+  </si>
+  <si>
+    <t>Offline 14</t>
+  </si>
+  <si>
+    <t>Offline 15</t>
+  </si>
+  <si>
+    <t>Offline 16</t>
+  </si>
+  <si>
+    <t>Online 3</t>
+  </si>
+  <si>
+    <t>Offline 17</t>
   </si>
 </sst>
 </file>
@@ -383,7 +398,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -666,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,33 +1114,129 @@
       <c r="N18" s="12"/>
     </row>
     <row r="19" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="22">
+      <c r="A19" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="18">
         <v>2</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="19">
         <v>43962</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="26">
         <v>2</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="28"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <f>SUM(B4:B19)</f>
-        <v>58</v>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="13"/>
+    </row>
+    <row r="20" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="18">
+        <v>2</v>
+      </c>
+      <c r="C20" s="19">
+        <v>43993</v>
+      </c>
+      <c r="D20" s="26">
+        <v>4</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="12"/>
+    </row>
+    <row r="21" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="18">
+        <v>6</v>
+      </c>
+      <c r="C21" s="19">
+        <v>44023</v>
+      </c>
+      <c r="D21" s="26">
+        <v>6</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="12"/>
+    </row>
+    <row r="22" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="18">
+        <v>4</v>
+      </c>
+      <c r="C22" s="19">
+        <v>44085</v>
+      </c>
+      <c r="D22" s="26">
+        <v>6</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="12"/>
+    </row>
+    <row r="23" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="22">
+        <v>6</v>
+      </c>
+      <c r="C23" s="23">
+        <v>44176</v>
+      </c>
+      <c r="D23" s="24">
+        <v>6</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="28"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f>SUM(B4:B23)</f>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Modified]: Meeting bar chart
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Báo Cáo Team/General/meeting_grant.xlsx
+++ b/ToDoApp-Doc/Báo Cáo Team/General/meeting_grant.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Offline 1</t>
   </si>
@@ -162,6 +162,60 @@
   </si>
   <si>
     <t>Offline 17</t>
+  </si>
+  <si>
+    <t>Offline 18</t>
+  </si>
+  <si>
+    <t>13/11/2020</t>
+  </si>
+  <si>
+    <t>Offline 19</t>
+  </si>
+  <si>
+    <t>14/11/2020</t>
+  </si>
+  <si>
+    <t>Online 4</t>
+  </si>
+  <si>
+    <t>16/11/2020</t>
+  </si>
+  <si>
+    <t>Online 5</t>
+  </si>
+  <si>
+    <t>17/11/2020</t>
+  </si>
+  <si>
+    <t>Offline 20</t>
+  </si>
+  <si>
+    <t>19/11/2020</t>
+  </si>
+  <si>
+    <t>Offline 21</t>
+  </si>
+  <si>
+    <t>20/11/2020</t>
+  </si>
+  <si>
+    <t>Offline 22</t>
+  </si>
+  <si>
+    <t>21/11/2020</t>
+  </si>
+  <si>
+    <t>Online 6</t>
+  </si>
+  <si>
+    <t>24/11/2020</t>
+  </si>
+  <si>
+    <t>Offline 23</t>
+  </si>
+  <si>
+    <t>26/11/2020</t>
   </si>
 </sst>
 </file>
@@ -338,9 +392,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -377,29 +428,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -681,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,31 +750,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -755,16 +809,16 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <v>4</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <v>6</v>
       </c>
       <c r="E4" s="2"/>
@@ -779,16 +833,16 @@
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>6</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>43900</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <v>4</v>
       </c>
       <c r="E5" s="2"/>
@@ -803,16 +857,16 @@
       <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="18">
-        <v>2</v>
-      </c>
-      <c r="C6" s="19">
+      <c r="A6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="17">
+        <v>2</v>
+      </c>
+      <c r="C6" s="18">
         <v>44053</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="15">
         <v>7</v>
       </c>
       <c r="E6" s="2"/>
@@ -827,16 +881,16 @@
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="18">
-        <v>2</v>
-      </c>
-      <c r="C7" s="19">
+      <c r="B7" s="17">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
         <v>44094</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <v>8</v>
       </c>
       <c r="E7" s="2"/>
@@ -850,16 +904,16 @@
       <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="17">
         <v>6</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="18">
         <v>44114</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="15">
         <v>4</v>
       </c>
       <c r="E8" s="2"/>
@@ -874,352 +928,352 @@
       <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="18">
-        <v>2</v>
-      </c>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="17">
+        <v>2</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <v>5</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="11"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <v>6</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="15">
         <v>5</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="12"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="11"/>
     </row>
     <row r="11" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>2.5</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="15">
         <v>6.5</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="13"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <v>2.5</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="15">
         <v>4.5</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="11"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="18">
-        <v>2</v>
-      </c>
-      <c r="C13" s="19" t="s">
+      <c r="B13" s="17">
+        <v>2</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="21">
         <v>4</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="12"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="17">
         <v>6</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="21">
         <v>6</v>
       </c>
-      <c r="E14" s="9"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="12"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="17">
         <v>5</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="21">
         <v>7</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="8"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="12"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="18">
-        <v>2</v>
-      </c>
-      <c r="C16" s="19" t="s">
+      <c r="B16" s="17">
+        <v>2</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="21">
         <v>6</v>
       </c>
-      <c r="E16" s="9"/>
+      <c r="E16" s="8"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="11"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="10"/>
     </row>
     <row r="17" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="18">
-        <v>2</v>
-      </c>
-      <c r="C17" s="19" t="s">
+      <c r="B17" s="17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="26">
-        <v>2</v>
-      </c>
-      <c r="E17" s="9"/>
+      <c r="D17" s="21">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="9"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="12"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="11"/>
     </row>
     <row r="18" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="17">
         <v>6</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="26">
-        <v>2</v>
-      </c>
-      <c r="E18" s="9"/>
+      <c r="D18" s="21">
+        <v>2</v>
+      </c>
+      <c r="E18" s="8"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="12"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="11"/>
     </row>
     <row r="19" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="18">
-        <v>2</v>
-      </c>
-      <c r="C19" s="19">
+      <c r="B19" s="17">
+        <v>2</v>
+      </c>
+      <c r="C19" s="18">
         <v>43962</v>
       </c>
-      <c r="D19" s="26">
-        <v>2</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
+      <c r="D19" s="21">
+        <v>2</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
-      <c r="N19" s="13"/>
+      <c r="N19" s="12"/>
     </row>
     <row r="20" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="18">
-        <v>2</v>
-      </c>
-      <c r="C20" s="19">
+      <c r="B20" s="17">
+        <v>2</v>
+      </c>
+      <c r="C20" s="18">
         <v>43993</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="21">
         <v>4</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="12"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="11"/>
     </row>
     <row r="21" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>6</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="18">
         <v>44023</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="21">
         <v>6</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
       <c r="L21" s="7"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="12"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="11"/>
     </row>
     <row r="22" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <v>4</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="18">
         <v>44085</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="21">
         <v>6</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
       <c r="L22" s="7"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="12"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="11"/>
     </row>
     <row r="23" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="22">
-        <v>2</v>
-      </c>
-      <c r="C23" s="23">
+      <c r="B23" s="17">
+        <v>2</v>
+      </c>
+      <c r="C23" s="18">
         <v>44176</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="21">
         <v>6</v>
       </c>
       <c r="E23" s="8"/>
@@ -1229,14 +1283,252 @@
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
-      <c r="L23" s="25"/>
+      <c r="L23" s="7"/>
       <c r="M23" s="8"/>
-      <c r="N23" s="27"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <f>SUM(B4:B23)</f>
-        <v>72</v>
+      <c r="N23" s="11"/>
+    </row>
+    <row r="24" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="17">
+        <v>2</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="11"/>
+    </row>
+    <row r="25" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="17">
+        <v>6</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="17">
+        <v>5</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="21"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="17">
+        <v>4</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="11"/>
+    </row>
+    <row r="28" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="17">
+        <v>2</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="21"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="11"/>
+    </row>
+    <row r="29" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="17">
+        <v>2</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="11"/>
+    </row>
+    <row r="30" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="17">
+        <v>6</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="21"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="11"/>
+    </row>
+    <row r="31" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="17">
+        <v>3</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="21"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="11"/>
+    </row>
+    <row r="32" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="17">
+        <v>2</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="21"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="11"/>
+    </row>
+    <row r="33" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="28"/>
+    </row>
+    <row r="34" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="25">
+        <v>2</v>
+      </c>
+      <c r="C34" s="26">
+        <v>44176</v>
+      </c>
+      <c r="D34" s="27">
+        <v>6</v>
+      </c>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="28"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f>SUM(B4:B32)</f>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>